<commit_message>
Gradle object and Gradle object
</commit_message>
<xml_diff>
--- a/me/3.Gradle-under-the-hood.xlsx
+++ b/me/3.Gradle-under-the-hood.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Gradle\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16FAD80-BD77-49BE-A110-B153B26D9E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3919B962-D68A-42D8-B595-D5C059686539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gradle Object Model" sheetId="1" r:id="rId1"/>
     <sheet name="Gradle Lifecycle" sheetId="2" r:id="rId2"/>
     <sheet name="Gradle Initialization Phase" sheetId="3" r:id="rId3"/>
+    <sheet name="GradleObjectModeAndGradleObject" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="108">
   <si>
     <t>構成</t>
   </si>
@@ -269,6 +270,222 @@
   </si>
   <si>
     <t>*/</t>
+  </si>
+  <si>
+    <t>logger.info "&gt;&gt;&gt; build.gradle: $project.gradle.gradleVersion"</t>
+  </si>
+  <si>
+    <t>logger.info "&gt;&gt;&gt; build.gradle: $project.gradle.gradleHomeDir"</t>
+  </si>
+  <si>
+    <t>logger.info "&gt;&gt;&gt; build.gradle: $project.gradle.gradleUserHomeDir"</t>
+  </si>
+  <si>
+    <t>in build.gradle file we are actually accessing the project object</t>
+  </si>
+  <si>
+    <t>gradle(timestamps())</t>
+  </si>
+  <si>
+    <t>code(build.gradle for having Project object as delegate)</t>
+  </si>
+  <si>
+    <t>logger.info "&gt;&gt;&gt; settings.gradle: $gradle.gradleVersion"</t>
+  </si>
+  <si>
+    <t>logger.info "&gt;&gt;&gt; settings.gradle: $gradle.gradleHomeDir"</t>
+  </si>
+  <si>
+    <t>logger.info "&gt;&gt;&gt; settings.gradle: $gradle.gradleUserHomeDir"</t>
+  </si>
+  <si>
+    <t>   def df = new SimpleDateFormat("yyyy-MM-dd'T'HH:mm:ss'Z'")</t>
+  </si>
+  <si>
+    <t>   df.setTimeZone(TimeZone.getTimeZone("UTC"))</t>
+  </si>
+  <si>
+    <t>   return df.format(new Date())</t>
+  </si>
+  <si>
+    <t>println "&gt;&gt;&gt; another.gradle --&gt; This is executed during the initialization phase  - timestamp @ ${gradle.timestamp()}"</t>
+  </si>
+  <si>
+    <t>logger.info "&gt;&gt;&gt; another.gradle: $gradleVersion"</t>
+  </si>
+  <si>
+    <t>logger.info "&gt;&gt;&gt; another.gradle: $gradleHomeDir"</t>
+  </si>
+  <si>
+    <t>logger.info "&gt;&gt;&gt; another.gradle: $gradleUserHomeDir"</t>
+  </si>
+  <si>
+    <t>println "&gt;&gt;&gt; init.gradle --&gt; This is executed during the initialization phase  - timestamp @ ${gradle.timestamp()}"</t>
+  </si>
+  <si>
+    <t>logger.info "&gt;&gt;&gt; init.gradle: $gradleVersion"</t>
+  </si>
+  <si>
+    <t>logger.info "&gt;&gt;&gt; init.gradle: $gradleHomeDir"</t>
+  </si>
+  <si>
+    <t>logger.info "&gt;&gt;&gt; init.gradle: $gradleUserHomeDir"</t>
+  </si>
+  <si>
+    <t>println "&gt;&gt;&gt; zingAnother.gradle --&gt; This is executed during the initialization phase  - timestamp @ ${gradle.timestamp()}"</t>
+  </si>
+  <si>
+    <t>logger.info "&gt;&gt;&gt; zingAnother.gradle: $gradleVersion"</t>
+  </si>
+  <si>
+    <t>logger.info "&gt;&gt;&gt; zingAnother.gradle: $gradleHomeDir"</t>
+  </si>
+  <si>
+    <t>logger.info "&gt;&gt;&gt; zingAnother.gradle: $gradleUserHomeDir"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">we are accessing </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>delicate object of project(gradle), then the property of</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">When we run build.gradle Gradle actually instantiate an object that </t>
+  </si>
+  <si>
+    <t>and methods. We also can access to another object called the delegate</t>
+  </si>
+  <si>
+    <t>delegate can change depending on which part of the build lifecycle we</t>
+  </si>
+  <si>
+    <t>happen to be in. For example we are in the actual configuration phase</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">implements the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Script</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> interface. We can access whole bunch of properties</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">and we are working on our build gradle file, delegate to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Project</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> interface</t>
+    </r>
+  </si>
+  <si>
+    <t>So in build.gradle file we can access to Script interface(properties and methods)</t>
+  </si>
+  <si>
+    <t>and we can access to delegate which is Project object(properties and methods)</t>
+  </si>
+  <si>
+    <t>settings.gradle: Can access to Script and Settings object</t>
+  </si>
+  <si>
+    <t>ini.gradle: Can access to Script and Gradle object</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">so we do not have to write the full </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>project.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>gradle.timestamp() means</t>
+    </r>
+  </si>
+  <si>
+    <t>https://docs.gradle.org/4.3/dsl/org.gradle.api.invocation.Gradle.html</t>
+  </si>
+  <si>
+    <t>We can write in a shorthand by removing the reference to project:</t>
+  </si>
+  <si>
+    <t>$gradle.gradleVersion</t>
+  </si>
+  <si>
+    <t>$gradle.gradleHomeDir</t>
+  </si>
+  <si>
+    <t>$gradle.gradleUserHomeDir</t>
+  </si>
+  <si>
+    <t>We can remove the reference to delegate object which is Gradle and we can access properties directly</t>
+  </si>
+  <si>
+    <t>We can write in a shorthand by removing the reference to settings:</t>
+  </si>
+  <si>
+    <t>$settings.gradle.gradleVersion</t>
+  </si>
+  <si>
+    <t>$settings.gradle.gradleHomeDir</t>
+  </si>
+  <si>
+    <t>$settings.gradle.gradleUserHomeDir</t>
   </si>
 </sst>
 </file>
@@ -397,7 +614,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -412,8 +629,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -981,6 +1199,579 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>380999</xdr:colOff>
+      <xdr:row>161</xdr:row>
+      <xdr:rowOff>162763</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9D57B6D-FE53-31F6-E3C7-4CFDAE5EFDEB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="676274" y="14373225"/>
+          <a:ext cx="9458325" cy="4839538"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>106972</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{022E2E7B-D0C8-4136-89A4-6F1035501C1B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="733425" y="476250"/>
+          <a:ext cx="7772400" cy="4583722"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7253751-B16F-AA49-E206-16AD6818EEBE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="7743825" y="1476375"/>
+          <a:ext cx="4114800" cy="133350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>52723</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DE04858-A23D-08AA-BA14-6F8AC82A21F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="698046" y="5791201"/>
+          <a:ext cx="11317061" cy="5691522"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{020A7AA9-02A6-9218-F7B8-374898424A4C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7105650" y="4133850"/>
+          <a:ext cx="4086225" cy="6819900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{257171BF-2BBC-9BFC-6014-29B68B7C3AAA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7667625" y="1609725"/>
+          <a:ext cx="3028950" cy="9334500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>257736</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>56029</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>403412</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86889D55-5E2C-6F94-7A49-FDDAD1E84D2D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3283324" y="10152529"/>
+          <a:ext cx="145676" cy="7664824"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>392206</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>145676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>560294</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A92C804-17D4-42AA-B854-964C95F5E6BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3417794" y="10623176"/>
+          <a:ext cx="168088" cy="7384677"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>582706</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>246529</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12CBC432-DB4F-8A69-A804-5C9D58E7ECC9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3608294" y="11116235"/>
+          <a:ext cx="268941" cy="6499412"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>448235</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>168088</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>448235</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>145676</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11E71FB4-C925-F7DC-0037-D9AE6EC98225}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4684059" y="3978088"/>
+          <a:ext cx="6051176" cy="2644588"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>56029</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>145676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>33618</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>100853</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88F60142-95BA-B258-2368-2A85CA136AB4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4291853" y="17671676"/>
+          <a:ext cx="4213412" cy="717177"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1246,7 +2037,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:S139"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M44" sqref="M44"/>
     </sheetView>
   </sheetViews>
@@ -1784,8 +2575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADAB4451-9FDF-4CEE-93B1-D1BDB7125C3E}">
   <dimension ref="A3:P22"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="R38" sqref="R38"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1828,10 +2619,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA13E3DA-3B48-4BFF-A04C-72AA6128C594}">
-  <dimension ref="A3:Q74"/>
+  <dimension ref="A3:P74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I78" sqref="I78"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2216,114 +3007,44 @@
       <c r="B55" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="14"/>
-      <c r="K55" s="14"/>
-      <c r="L55" s="14"/>
       <c r="M55" s="6"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B56" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
-      <c r="J56" s="14"/>
-      <c r="K56" s="14"/>
-      <c r="L56" s="14"/>
       <c r="M56" s="6"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B57" s="5"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
-      <c r="J57" s="14"/>
-      <c r="K57" s="14"/>
-      <c r="L57" s="14"/>
       <c r="M57" s="6"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B58" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="14"/>
-      <c r="G58" s="14"/>
-      <c r="H58" s="14"/>
-      <c r="I58" s="14"/>
-      <c r="J58" s="14"/>
-      <c r="K58" s="14"/>
-      <c r="L58" s="14"/>
       <c r="M58" s="6"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B59" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="14"/>
-      <c r="F59" s="14"/>
-      <c r="G59" s="14"/>
-      <c r="H59" s="14"/>
-      <c r="I59" s="14"/>
-      <c r="J59" s="14"/>
-      <c r="K59" s="14"/>
-      <c r="L59" s="14"/>
       <c r="M59" s="6"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B60" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="14"/>
-      <c r="G60" s="14"/>
-      <c r="H60" s="14"/>
-      <c r="I60" s="14"/>
-      <c r="J60" s="14"/>
-      <c r="K60" s="14"/>
-      <c r="L60" s="14"/>
       <c r="M60" s="6"/>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B61" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C61" s="14"/>
-      <c r="D61" s="14"/>
-      <c r="E61" s="14"/>
-      <c r="F61" s="14"/>
-      <c r="G61" s="14"/>
-      <c r="H61" s="14"/>
-      <c r="I61" s="14"/>
-      <c r="J61" s="14"/>
-      <c r="K61" s="14"/>
-      <c r="L61" s="14"/>
       <c r="M61" s="6"/>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B62" s="15" t="s">
+      <c r="B62" s="14" t="s">
         <v>59</v>
       </c>
       <c r="C62" s="9"/>
@@ -2338,7 +3059,7 @@
       <c r="L62" s="9"/>
       <c r="M62" s="10"/>
     </row>
-    <row r="65" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
         <v>56</v>
       </c>
@@ -2356,153 +3077,40 @@
       <c r="N65" s="3"/>
       <c r="O65" s="3"/>
       <c r="P65" s="4"/>
-      <c r="Q65" s="14"/>
-    </row>
-    <row r="66" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B66" s="5"/>
-      <c r="C66" s="14"/>
-      <c r="D66" s="14"/>
-      <c r="E66" s="14"/>
-      <c r="F66" s="14"/>
-      <c r="G66" s="14"/>
-      <c r="H66" s="14"/>
-      <c r="I66" s="14"/>
-      <c r="J66" s="14"/>
-      <c r="K66" s="14"/>
-      <c r="L66" s="14"/>
-      <c r="M66" s="14"/>
-      <c r="N66" s="14"/>
-      <c r="O66" s="14"/>
       <c r="P66" s="6"/>
-      <c r="Q66" s="14"/>
-    </row>
-    <row r="67" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B67" s="5"/>
-      <c r="C67" s="14"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="14"/>
-      <c r="F67" s="14"/>
-      <c r="G67" s="14"/>
-      <c r="H67" s="14"/>
-      <c r="I67" s="14"/>
-      <c r="J67" s="14"/>
-      <c r="K67" s="14"/>
-      <c r="L67" s="14"/>
-      <c r="M67" s="14"/>
-      <c r="N67" s="14"/>
-      <c r="O67" s="14"/>
       <c r="P67" s="6"/>
-      <c r="Q67" s="14"/>
-    </row>
-    <row r="68" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B68" s="5"/>
-      <c r="C68" s="14"/>
-      <c r="D68" s="14"/>
-      <c r="E68" s="14"/>
-      <c r="F68" s="14"/>
-      <c r="G68" s="14"/>
-      <c r="H68" s="14"/>
-      <c r="I68" s="14"/>
-      <c r="J68" s="14"/>
-      <c r="K68" s="14"/>
-      <c r="L68" s="14"/>
-      <c r="M68" s="14"/>
-      <c r="N68" s="14"/>
-      <c r="O68" s="14"/>
       <c r="P68" s="6"/>
-      <c r="Q68" s="14"/>
-    </row>
-    <row r="69" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B69" s="5"/>
-      <c r="C69" s="14"/>
-      <c r="D69" s="14"/>
-      <c r="E69" s="14"/>
-      <c r="F69" s="14"/>
-      <c r="G69" s="14"/>
-      <c r="H69" s="14"/>
-      <c r="I69" s="14"/>
-      <c r="J69" s="14"/>
-      <c r="K69" s="14"/>
-      <c r="L69" s="14"/>
-      <c r="M69" s="14"/>
-      <c r="N69" s="14"/>
-      <c r="O69" s="14"/>
       <c r="P69" s="6"/>
-      <c r="Q69" s="14"/>
-    </row>
-    <row r="70" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B70" s="5"/>
-      <c r="C70" s="14"/>
-      <c r="D70" s="14"/>
-      <c r="E70" s="14"/>
-      <c r="F70" s="14"/>
-      <c r="G70" s="14"/>
-      <c r="H70" s="14"/>
-      <c r="I70" s="14"/>
-      <c r="J70" s="14"/>
-      <c r="K70" s="14"/>
-      <c r="L70" s="14"/>
-      <c r="M70" s="14"/>
-      <c r="N70" s="14"/>
-      <c r="O70" s="14"/>
       <c r="P70" s="6"/>
-      <c r="Q70" s="14"/>
-    </row>
-    <row r="71" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B71" s="5"/>
-      <c r="C71" s="14"/>
-      <c r="D71" s="14"/>
-      <c r="E71" s="14"/>
-      <c r="F71" s="14"/>
-      <c r="G71" s="14"/>
-      <c r="H71" s="14"/>
-      <c r="I71" s="14"/>
-      <c r="J71" s="14"/>
-      <c r="K71" s="14"/>
-      <c r="L71" s="14"/>
-      <c r="M71" s="14"/>
-      <c r="N71" s="14"/>
-      <c r="O71" s="14"/>
       <c r="P71" s="6"/>
-      <c r="Q71" s="14"/>
-    </row>
-    <row r="72" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B72" s="5"/>
-      <c r="C72" s="14"/>
-      <c r="D72" s="14"/>
-      <c r="E72" s="14"/>
-      <c r="F72" s="14"/>
-      <c r="G72" s="14"/>
-      <c r="H72" s="14"/>
-      <c r="I72" s="14"/>
-      <c r="J72" s="14"/>
-      <c r="K72" s="14"/>
-      <c r="L72" s="14"/>
-      <c r="M72" s="14"/>
-      <c r="N72" s="14"/>
-      <c r="O72" s="14"/>
       <c r="P72" s="6"/>
-      <c r="Q72" s="14"/>
-    </row>
-    <row r="73" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B73" s="5"/>
-      <c r="C73" s="14"/>
-      <c r="D73" s="14"/>
-      <c r="E73" s="14"/>
-      <c r="F73" s="14"/>
-      <c r="G73" s="14"/>
-      <c r="H73" s="14"/>
-      <c r="I73" s="14"/>
-      <c r="J73" s="14"/>
-      <c r="K73" s="14"/>
-      <c r="L73" s="14"/>
-      <c r="M73" s="14"/>
-      <c r="N73" s="14"/>
-      <c r="O73" s="14"/>
       <c r="P73" s="6"/>
-      <c r="Q73" s="14"/>
-    </row>
-    <row r="74" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B74" s="8"/>
       <c r="C74" s="9"/>
       <c r="D74" s="9"/>
@@ -2518,7 +3126,1454 @@
       <c r="N74" s="9"/>
       <c r="O74" s="9"/>
       <c r="P74" s="10"/>
-      <c r="Q74" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A38C079-6877-4B4A-A623-D287188FE0EB}">
+  <dimension ref="A4:Y135"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S109" sqref="S109"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="O21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+      <c r="T29" s="4"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B30" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16"/>
+      <c r="P30" s="16"/>
+      <c r="Q30" s="16"/>
+      <c r="R30" s="16"/>
+      <c r="S30" s="16"/>
+      <c r="T30" s="6"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B31" s="5"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="16"/>
+      <c r="P31" s="16"/>
+      <c r="Q31" s="16"/>
+      <c r="R31" s="16"/>
+      <c r="S31" s="16"/>
+      <c r="T31" s="6"/>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="16"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="16"/>
+      <c r="P32" s="16"/>
+      <c r="Q32" s="16"/>
+      <c r="R32" s="16"/>
+      <c r="S32" s="16"/>
+      <c r="T32" s="6"/>
+    </row>
+    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B33" s="5"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="16"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="16"/>
+      <c r="Q33" s="16"/>
+      <c r="R33" s="16"/>
+      <c r="S33" s="16"/>
+      <c r="T33" s="6"/>
+    </row>
+    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B34" s="5"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="16"/>
+      <c r="R34" s="16"/>
+      <c r="S34" s="16"/>
+      <c r="T34" s="6"/>
+    </row>
+    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B35" s="5"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="16"/>
+      <c r="N35" s="16"/>
+      <c r="O35" s="16"/>
+      <c r="P35" s="16"/>
+      <c r="Q35" s="16"/>
+      <c r="R35" s="16"/>
+      <c r="S35" s="16"/>
+      <c r="T35" s="6"/>
+    </row>
+    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B36" s="5"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="16"/>
+      <c r="N36" s="16"/>
+      <c r="O36" s="16"/>
+      <c r="P36" s="16"/>
+      <c r="Q36" s="16"/>
+      <c r="R36" s="16"/>
+      <c r="S36" s="16"/>
+      <c r="T36" s="6"/>
+    </row>
+    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B37" s="5"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="16"/>
+      <c r="K37" s="16"/>
+      <c r="L37" s="16"/>
+      <c r="M37" s="16"/>
+      <c r="N37" s="16"/>
+      <c r="O37" s="16"/>
+      <c r="P37" s="16"/>
+      <c r="Q37" s="16"/>
+      <c r="R37" s="16"/>
+      <c r="S37" s="16"/>
+      <c r="T37" s="6"/>
+    </row>
+    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B38" s="5"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
+      <c r="M38" s="16"/>
+      <c r="N38" s="16"/>
+      <c r="O38" s="16"/>
+      <c r="P38" s="16"/>
+      <c r="Q38" s="16"/>
+      <c r="R38" s="16"/>
+      <c r="S38" s="16"/>
+      <c r="T38" s="6"/>
+    </row>
+    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B39" s="5"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16"/>
+      <c r="M39" s="16"/>
+      <c r="N39" s="16"/>
+      <c r="O39" s="16"/>
+      <c r="P39" s="16"/>
+      <c r="Q39" s="16"/>
+      <c r="R39" s="16"/>
+      <c r="S39" s="16"/>
+      <c r="T39" s="6"/>
+    </row>
+    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B40" s="5"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="16"/>
+      <c r="M40" s="16"/>
+      <c r="N40" s="16"/>
+      <c r="O40" s="16"/>
+      <c r="P40" s="16"/>
+      <c r="Q40" s="16"/>
+      <c r="R40" s="16"/>
+      <c r="S40" s="16"/>
+      <c r="T40" s="6"/>
+    </row>
+    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B41" s="5"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16"/>
+      <c r="J41" s="16"/>
+      <c r="K41" s="16"/>
+      <c r="L41" s="16"/>
+      <c r="M41" s="16"/>
+      <c r="N41" s="16"/>
+      <c r="O41" s="16"/>
+      <c r="P41" s="16"/>
+      <c r="Q41" s="16"/>
+      <c r="R41" s="16"/>
+      <c r="S41" s="16"/>
+      <c r="T41" s="6"/>
+    </row>
+    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B42" s="5"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
+      <c r="J42" s="16"/>
+      <c r="K42" s="16"/>
+      <c r="L42" s="16"/>
+      <c r="M42" s="16"/>
+      <c r="N42" s="16"/>
+      <c r="O42" s="16"/>
+      <c r="P42" s="16"/>
+      <c r="Q42" s="16"/>
+      <c r="R42" s="16"/>
+      <c r="S42" s="16"/>
+      <c r="T42" s="6"/>
+    </row>
+    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B43" s="5"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
+      <c r="J43" s="16"/>
+      <c r="K43" s="16"/>
+      <c r="L43" s="16"/>
+      <c r="M43" s="16"/>
+      <c r="N43" s="16"/>
+      <c r="O43" s="16"/>
+      <c r="P43" s="16"/>
+      <c r="Q43" s="16"/>
+      <c r="R43" s="16"/>
+      <c r="S43" s="16"/>
+      <c r="T43" s="6"/>
+    </row>
+    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B44" s="5"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="16"/>
+      <c r="J44" s="16"/>
+      <c r="K44" s="16"/>
+      <c r="L44" s="16"/>
+      <c r="M44" s="16"/>
+      <c r="N44" s="16"/>
+      <c r="O44" s="16"/>
+      <c r="P44" s="16"/>
+      <c r="Q44" s="16"/>
+      <c r="R44" s="16"/>
+      <c r="S44" s="16"/>
+      <c r="T44" s="6"/>
+    </row>
+    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B45" s="5"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
+      <c r="J45" s="16"/>
+      <c r="K45" s="16"/>
+      <c r="L45" s="16"/>
+      <c r="M45" s="16"/>
+      <c r="N45" s="16"/>
+      <c r="O45" s="16"/>
+      <c r="P45" s="16"/>
+      <c r="Q45" s="16"/>
+      <c r="R45" s="16"/>
+      <c r="S45" s="16"/>
+      <c r="T45" s="6"/>
+    </row>
+    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B46" s="5"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="16"/>
+      <c r="J46" s="16"/>
+      <c r="K46" s="16"/>
+      <c r="L46" s="16"/>
+      <c r="M46" s="16"/>
+      <c r="N46" s="16"/>
+      <c r="O46" s="16"/>
+      <c r="P46" s="16"/>
+      <c r="Q46" s="16"/>
+      <c r="R46" s="16"/>
+      <c r="S46" s="16"/>
+      <c r="T46" s="6"/>
+    </row>
+    <row r="47" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B47" s="5"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="16"/>
+      <c r="K47" s="16"/>
+      <c r="L47" s="16"/>
+      <c r="M47" s="16"/>
+      <c r="N47" s="16"/>
+      <c r="O47" s="16"/>
+      <c r="P47" s="16"/>
+      <c r="Q47" s="16"/>
+      <c r="R47" s="16"/>
+      <c r="S47" s="16"/>
+      <c r="T47" s="6"/>
+    </row>
+    <row r="48" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B48" s="5"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
+      <c r="I48" s="16"/>
+      <c r="J48" s="16"/>
+      <c r="K48" s="16"/>
+      <c r="L48" s="16"/>
+      <c r="M48" s="16"/>
+      <c r="N48" s="16"/>
+      <c r="O48" s="16"/>
+      <c r="P48" s="16"/>
+      <c r="Q48" s="16"/>
+      <c r="R48" s="16"/>
+      <c r="S48" s="16"/>
+      <c r="T48" s="6"/>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B49" s="5"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="16"/>
+      <c r="I49" s="16"/>
+      <c r="J49" s="16"/>
+      <c r="K49" s="16"/>
+      <c r="L49" s="16"/>
+      <c r="M49" s="16"/>
+      <c r="N49" s="16"/>
+      <c r="O49" s="16"/>
+      <c r="P49" s="16"/>
+      <c r="Q49" s="16"/>
+      <c r="R49" s="16"/>
+      <c r="S49" s="16"/>
+      <c r="T49" s="6"/>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B50" s="5"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="16"/>
+      <c r="H50" s="16"/>
+      <c r="I50" s="16"/>
+      <c r="J50" s="16"/>
+      <c r="K50" s="16"/>
+      <c r="L50" s="16"/>
+      <c r="M50" s="16"/>
+      <c r="N50" s="16"/>
+      <c r="O50" s="16"/>
+      <c r="P50" s="16"/>
+      <c r="Q50" s="16"/>
+      <c r="R50" s="16"/>
+      <c r="S50" s="16"/>
+      <c r="T50" s="6"/>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B51" s="5"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="16"/>
+      <c r="H51" s="16"/>
+      <c r="I51" s="16"/>
+      <c r="J51" s="16"/>
+      <c r="K51" s="16"/>
+      <c r="L51" s="16"/>
+      <c r="M51" s="16"/>
+      <c r="N51" s="16"/>
+      <c r="O51" s="16"/>
+      <c r="P51" s="16"/>
+      <c r="Q51" s="16"/>
+      <c r="R51" s="16"/>
+      <c r="S51" s="16"/>
+      <c r="T51" s="6"/>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B52" s="5"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16"/>
+      <c r="I52" s="16"/>
+      <c r="J52" s="16"/>
+      <c r="K52" s="16"/>
+      <c r="L52" s="16"/>
+      <c r="M52" s="16"/>
+      <c r="N52" s="16"/>
+      <c r="O52" s="16"/>
+      <c r="P52" s="16"/>
+      <c r="Q52" s="16"/>
+      <c r="R52" s="16"/>
+      <c r="S52" s="16"/>
+      <c r="T52" s="6"/>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B53" s="5"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="16"/>
+      <c r="E53" s="16"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="16"/>
+      <c r="I53" s="16"/>
+      <c r="J53" s="16"/>
+      <c r="K53" s="16"/>
+      <c r="L53" s="16"/>
+      <c r="M53" s="16"/>
+      <c r="N53" s="16"/>
+      <c r="O53" s="16"/>
+      <c r="P53" s="16"/>
+      <c r="Q53" s="16"/>
+      <c r="R53" s="16"/>
+      <c r="S53" s="16"/>
+      <c r="T53" s="6"/>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B54" s="5"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="16"/>
+      <c r="E54" s="16"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="16"/>
+      <c r="H54" s="16"/>
+      <c r="I54" s="16"/>
+      <c r="J54" s="16"/>
+      <c r="K54" s="16"/>
+      <c r="L54" s="16"/>
+      <c r="M54" s="16"/>
+      <c r="N54" s="16"/>
+      <c r="O54" s="16"/>
+      <c r="P54" s="16"/>
+      <c r="Q54" s="16"/>
+      <c r="R54" s="16"/>
+      <c r="S54" s="16"/>
+      <c r="T54" s="6"/>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B55" s="5"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="16"/>
+      <c r="I55" s="16"/>
+      <c r="J55" s="16"/>
+      <c r="K55" s="16"/>
+      <c r="L55" s="16"/>
+      <c r="M55" s="16"/>
+      <c r="N55" s="16"/>
+      <c r="O55" s="16"/>
+      <c r="P55" s="16"/>
+      <c r="Q55" s="16"/>
+      <c r="R55" s="16"/>
+      <c r="S55" s="16"/>
+      <c r="T55" s="6"/>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B56" s="5"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
+      <c r="I56" s="16"/>
+      <c r="J56" s="16"/>
+      <c r="K56" s="16"/>
+      <c r="L56" s="16"/>
+      <c r="M56" s="16"/>
+      <c r="N56" s="16"/>
+      <c r="O56" s="16"/>
+      <c r="P56" s="16"/>
+      <c r="Q56" s="16"/>
+      <c r="R56" s="16"/>
+      <c r="S56" s="16"/>
+      <c r="T56" s="6"/>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B57" s="5"/>
+      <c r="C57" s="16"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="16"/>
+      <c r="F57" s="16"/>
+      <c r="G57" s="16"/>
+      <c r="H57" s="16"/>
+      <c r="I57" s="16"/>
+      <c r="J57" s="16"/>
+      <c r="K57" s="16"/>
+      <c r="L57" s="16"/>
+      <c r="M57" s="16"/>
+      <c r="N57" s="16"/>
+      <c r="O57" s="16"/>
+      <c r="P57" s="16"/>
+      <c r="Q57" s="16"/>
+      <c r="R57" s="16"/>
+      <c r="S57" s="16"/>
+      <c r="T57" s="6"/>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B58" s="5"/>
+      <c r="C58" s="16"/>
+      <c r="D58" s="16"/>
+      <c r="E58" s="16"/>
+      <c r="F58" s="16"/>
+      <c r="G58" s="16"/>
+      <c r="H58" s="16"/>
+      <c r="I58" s="16"/>
+      <c r="J58" s="16"/>
+      <c r="K58" s="16"/>
+      <c r="L58" s="16"/>
+      <c r="M58" s="16"/>
+      <c r="N58" s="16"/>
+      <c r="O58" s="16"/>
+      <c r="P58" s="16"/>
+      <c r="Q58" s="16"/>
+      <c r="R58" s="16"/>
+      <c r="S58" s="16"/>
+      <c r="T58" s="6"/>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B59" s="5"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="16"/>
+      <c r="E59" s="16"/>
+      <c r="F59" s="16"/>
+      <c r="G59" s="16"/>
+      <c r="H59" s="16"/>
+      <c r="I59" s="16"/>
+      <c r="J59" s="16"/>
+      <c r="K59" s="16"/>
+      <c r="L59" s="16"/>
+      <c r="M59" s="16"/>
+      <c r="N59" s="16"/>
+      <c r="O59" s="16"/>
+      <c r="P59" s="16"/>
+      <c r="Q59" s="16"/>
+      <c r="R59" s="16"/>
+      <c r="S59" s="16"/>
+      <c r="T59" s="6"/>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B60" s="5"/>
+      <c r="C60" s="16"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="16"/>
+      <c r="F60" s="16"/>
+      <c r="G60" s="16"/>
+      <c r="H60" s="16"/>
+      <c r="I60" s="16"/>
+      <c r="J60" s="16"/>
+      <c r="K60" s="16"/>
+      <c r="L60" s="16"/>
+      <c r="M60" s="16"/>
+      <c r="N60" s="16"/>
+      <c r="O60" s="16"/>
+      <c r="P60" s="16"/>
+      <c r="Q60" s="16"/>
+      <c r="R60" s="16"/>
+      <c r="S60" s="16"/>
+      <c r="T60" s="6"/>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B61" s="8"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="9"/>
+      <c r="H61" s="9"/>
+      <c r="I61" s="9"/>
+      <c r="J61" s="9"/>
+      <c r="K61" s="9"/>
+      <c r="L61" s="9"/>
+      <c r="M61" s="9"/>
+      <c r="N61" s="9"/>
+      <c r="O61" s="9"/>
+      <c r="P61" s="9"/>
+      <c r="Q61" s="9"/>
+      <c r="R61" s="9"/>
+      <c r="S61" s="9"/>
+      <c r="T61" s="10"/>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B65" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="4"/>
+    </row>
+    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B66" s="5"/>
+      <c r="C66" t="s">
+        <v>2</v>
+      </c>
+      <c r="I66" s="6"/>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B67" s="5"/>
+      <c r="D67" t="s">
+        <v>3</v>
+      </c>
+      <c r="I67" s="6"/>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B68" s="5"/>
+      <c r="E68" t="s">
+        <v>4</v>
+      </c>
+      <c r="I68" s="6"/>
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B69" s="5"/>
+      <c r="C69" t="s">
+        <v>5</v>
+      </c>
+      <c r="I69" s="6"/>
+    </row>
+    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B70" s="5"/>
+      <c r="C70" t="s">
+        <v>7</v>
+      </c>
+      <c r="I70" s="6"/>
+    </row>
+    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B71" s="5"/>
+      <c r="D71" t="s">
+        <v>8</v>
+      </c>
+      <c r="I71" s="6"/>
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B72" s="5"/>
+      <c r="E72" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="I72" s="6"/>
+      <c r="J72" t="s">
+        <v>6</v>
+      </c>
+      <c r="K72" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B73" s="5"/>
+      <c r="E73" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I73" s="6"/>
+      <c r="J73" t="s">
+        <v>6</v>
+      </c>
+      <c r="K73" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B74" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I74" s="6"/>
+    </row>
+    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B75" s="5"/>
+      <c r="C75" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I75" s="6"/>
+    </row>
+    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B76" s="5"/>
+      <c r="D76" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I76" s="6"/>
+      <c r="J76" t="s">
+        <v>6</v>
+      </c>
+      <c r="K76" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B77" s="5"/>
+      <c r="D77" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I77" s="6"/>
+      <c r="J77" t="s">
+        <v>6</v>
+      </c>
+      <c r="K77" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B78" s="5"/>
+      <c r="D78" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I78" s="6"/>
+      <c r="J78" t="s">
+        <v>6</v>
+      </c>
+      <c r="K78" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B79" s="8"/>
+      <c r="C79" s="9"/>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="9"/>
+      <c r="H79" s="9"/>
+      <c r="I79" s="10"/>
+    </row>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B83" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
+      <c r="H83" s="3"/>
+      <c r="I83" s="3"/>
+      <c r="J83" s="3"/>
+      <c r="K83" s="3"/>
+      <c r="L83" s="3"/>
+      <c r="M83" s="4"/>
+    </row>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B84" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="M84" s="6"/>
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B85" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M85" s="6"/>
+    </row>
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B86" s="5"/>
+      <c r="M86" s="6"/>
+    </row>
+    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B87" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M87" s="6"/>
+    </row>
+    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B88" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M88" s="6"/>
+    </row>
+    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B89" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M89" s="6"/>
+    </row>
+    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B90" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="M90" s="6"/>
+    </row>
+    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B91" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="M91" s="6"/>
+      <c r="N91" t="s">
+        <v>6</v>
+      </c>
+      <c r="O91" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B92" s="5"/>
+      <c r="M92" s="6"/>
+      <c r="O92" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B93" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="M93" s="6"/>
+      <c r="O93" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B94" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="M94" s="6"/>
+      <c r="O94" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B95" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C95" s="9"/>
+      <c r="D95" s="9"/>
+      <c r="E95" s="9"/>
+      <c r="F95" s="9"/>
+      <c r="G95" s="9"/>
+      <c r="H95" s="9"/>
+      <c r="I95" s="9"/>
+      <c r="J95" s="9"/>
+      <c r="K95" s="9"/>
+      <c r="L95" s="9"/>
+      <c r="M95" s="10"/>
+    </row>
+    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O96" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="P96" s="3"/>
+      <c r="Q96" s="3"/>
+      <c r="R96" s="3"/>
+      <c r="S96" s="3"/>
+      <c r="T96" s="3"/>
+      <c r="U96" s="4"/>
+    </row>
+    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O97" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="P97" s="16"/>
+      <c r="Q97" s="16"/>
+      <c r="R97" s="16"/>
+      <c r="S97" s="16"/>
+      <c r="T97" s="16"/>
+      <c r="U97" s="6"/>
+    </row>
+    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>53</v>
+      </c>
+      <c r="O98" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="P98" s="16"/>
+      <c r="Q98" s="16"/>
+      <c r="R98" s="16"/>
+      <c r="S98" s="16"/>
+      <c r="T98" s="16"/>
+      <c r="U98" s="6"/>
+    </row>
+    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B99" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="3"/>
+      <c r="F99" s="3"/>
+      <c r="G99" s="3"/>
+      <c r="H99" s="3"/>
+      <c r="I99" s="3"/>
+      <c r="J99" s="3"/>
+      <c r="K99" s="3"/>
+      <c r="L99" s="3"/>
+      <c r="M99" s="4"/>
+      <c r="O99" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="P99" s="9"/>
+      <c r="Q99" s="9"/>
+      <c r="R99" s="9"/>
+      <c r="S99" s="9"/>
+      <c r="T99" s="9"/>
+      <c r="U99" s="10"/>
+    </row>
+    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B100" s="5"/>
+      <c r="M100" s="6"/>
+      <c r="O100" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="P100" s="3"/>
+      <c r="Q100" s="3"/>
+      <c r="R100" s="3"/>
+      <c r="S100" s="3"/>
+      <c r="T100" s="3"/>
+      <c r="U100" s="4"/>
+    </row>
+    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B101" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="M101" s="6"/>
+      <c r="O101" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="P101" s="16"/>
+      <c r="Q101" s="16"/>
+      <c r="R101" s="16"/>
+      <c r="S101" s="16"/>
+      <c r="T101" s="16"/>
+      <c r="U101" s="6"/>
+    </row>
+    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B102" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="M102" s="6"/>
+      <c r="O102" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="P102" s="16"/>
+      <c r="Q102" s="16"/>
+      <c r="R102" s="16"/>
+      <c r="S102" s="16"/>
+      <c r="T102" s="16"/>
+      <c r="U102" s="6"/>
+    </row>
+    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B103" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C103" s="9"/>
+      <c r="D103" s="9"/>
+      <c r="E103" s="9"/>
+      <c r="F103" s="9"/>
+      <c r="G103" s="9"/>
+      <c r="H103" s="9"/>
+      <c r="I103" s="9"/>
+      <c r="J103" s="9"/>
+      <c r="K103" s="9"/>
+      <c r="L103" s="9"/>
+      <c r="M103" s="10"/>
+      <c r="O103" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="P103" s="9"/>
+      <c r="Q103" s="9"/>
+      <c r="R103" s="9"/>
+      <c r="S103" s="9"/>
+      <c r="T103" s="9"/>
+      <c r="U103" s="10"/>
+    </row>
+    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="107" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B107" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C107" s="3"/>
+      <c r="D107" s="3"/>
+      <c r="E107" s="3"/>
+      <c r="F107" s="3"/>
+      <c r="G107" s="3"/>
+      <c r="H107" s="3"/>
+      <c r="I107" s="3"/>
+      <c r="J107" s="3"/>
+      <c r="K107" s="3"/>
+      <c r="L107" s="3"/>
+      <c r="M107" s="4"/>
+    </row>
+    <row r="108" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B108" s="5"/>
+      <c r="M108" s="6"/>
+    </row>
+    <row r="109" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B109" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="M109" s="6"/>
+    </row>
+    <row r="110" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B110" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="M110" s="6"/>
+    </row>
+    <row r="111" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B111" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="M111" s="6"/>
+    </row>
+    <row r="112" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B112" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="M112" s="6"/>
+    </row>
+    <row r="113" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B113" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M113" s="6"/>
+    </row>
+    <row r="114" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B114" s="5"/>
+      <c r="M114" s="6"/>
+    </row>
+    <row r="115" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B115" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M115" s="6"/>
+    </row>
+    <row r="116" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B116" s="5"/>
+      <c r="M116" s="6"/>
+    </row>
+    <row r="117" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B117" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="M117" s="6"/>
+    </row>
+    <row r="118" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B118" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="M118" s="6"/>
+    </row>
+    <row r="119" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B119" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C119" s="9"/>
+      <c r="D119" s="9"/>
+      <c r="E119" s="9"/>
+      <c r="F119" s="9"/>
+      <c r="G119" s="9"/>
+      <c r="H119" s="9"/>
+      <c r="I119" s="9"/>
+      <c r="J119" s="9"/>
+      <c r="K119" s="9"/>
+      <c r="L119" s="9"/>
+      <c r="M119" s="10"/>
+    </row>
+    <row r="122" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="123" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B123" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C123" s="3"/>
+      <c r="D123" s="3"/>
+      <c r="E123" s="3"/>
+      <c r="F123" s="3"/>
+      <c r="G123" s="3"/>
+      <c r="H123" s="3"/>
+      <c r="I123" s="3"/>
+      <c r="J123" s="3"/>
+      <c r="K123" s="3"/>
+      <c r="L123" s="3"/>
+      <c r="M123" s="4"/>
+    </row>
+    <row r="124" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B124" s="5"/>
+      <c r="C124" s="16"/>
+      <c r="D124" s="16"/>
+      <c r="E124" s="16"/>
+      <c r="F124" s="16"/>
+      <c r="G124" s="16"/>
+      <c r="H124" s="16"/>
+      <c r="I124" s="16"/>
+      <c r="J124" s="16"/>
+      <c r="K124" s="16"/>
+      <c r="L124" s="16"/>
+      <c r="M124" s="6"/>
+      <c r="O124" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="P124" s="3"/>
+      <c r="Q124" s="3"/>
+      <c r="R124" s="3"/>
+      <c r="S124" s="3"/>
+      <c r="T124" s="3"/>
+      <c r="U124" s="3"/>
+      <c r="V124" s="3"/>
+      <c r="W124" s="3"/>
+      <c r="X124" s="3"/>
+      <c r="Y124" s="4"/>
+    </row>
+    <row r="125" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B125" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C125" s="16"/>
+      <c r="D125" s="16"/>
+      <c r="E125" s="16"/>
+      <c r="F125" s="16"/>
+      <c r="G125" s="16"/>
+      <c r="H125" s="16"/>
+      <c r="I125" s="16"/>
+      <c r="J125" s="16"/>
+      <c r="K125" s="16"/>
+      <c r="L125" s="16"/>
+      <c r="M125" s="6"/>
+      <c r="N125" t="s">
+        <v>6</v>
+      </c>
+      <c r="O125" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="P125" s="16"/>
+      <c r="Q125" s="16"/>
+      <c r="R125" s="16"/>
+      <c r="S125" s="16"/>
+      <c r="T125" s="16"/>
+      <c r="U125" s="16"/>
+      <c r="V125" s="16"/>
+      <c r="W125" s="16"/>
+      <c r="X125" s="16"/>
+      <c r="Y125" s="6"/>
+    </row>
+    <row r="126" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B126" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C126" s="16"/>
+      <c r="D126" s="16"/>
+      <c r="E126" s="16"/>
+      <c r="F126" s="16"/>
+      <c r="G126" s="16"/>
+      <c r="H126" s="16"/>
+      <c r="I126" s="16"/>
+      <c r="J126" s="16"/>
+      <c r="K126" s="16"/>
+      <c r="L126" s="16"/>
+      <c r="M126" s="6"/>
+      <c r="N126" t="s">
+        <v>6</v>
+      </c>
+      <c r="O126" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="P126" s="16"/>
+      <c r="Q126" s="16"/>
+      <c r="R126" s="16"/>
+      <c r="S126" s="16"/>
+      <c r="T126" s="16"/>
+      <c r="U126" s="16"/>
+      <c r="V126" s="16"/>
+      <c r="W126" s="16"/>
+      <c r="X126" s="16"/>
+      <c r="Y126" s="6"/>
+    </row>
+    <row r="127" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B127" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C127" s="9"/>
+      <c r="D127" s="9"/>
+      <c r="E127" s="9"/>
+      <c r="F127" s="9"/>
+      <c r="G127" s="9"/>
+      <c r="H127" s="9"/>
+      <c r="I127" s="9"/>
+      <c r="J127" s="9"/>
+      <c r="K127" s="9"/>
+      <c r="L127" s="9"/>
+      <c r="M127" s="10"/>
+      <c r="N127" t="s">
+        <v>6</v>
+      </c>
+      <c r="O127" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="P127" s="9"/>
+      <c r="Q127" s="9"/>
+      <c r="R127" s="9"/>
+      <c r="S127" s="9"/>
+      <c r="T127" s="9"/>
+      <c r="U127" s="9"/>
+      <c r="V127" s="9"/>
+      <c r="W127" s="9"/>
+      <c r="X127" s="9"/>
+      <c r="Y127" s="10"/>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B131" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C131" s="3"/>
+      <c r="D131" s="3"/>
+      <c r="E131" s="3"/>
+      <c r="F131" s="3"/>
+      <c r="G131" s="3"/>
+      <c r="H131" s="3"/>
+      <c r="I131" s="3"/>
+      <c r="J131" s="3"/>
+      <c r="K131" s="3"/>
+      <c r="L131" s="3"/>
+      <c r="M131" s="4"/>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B132" s="5"/>
+      <c r="M132" s="6"/>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B133" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="M133" s="6"/>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B134" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="M134" s="6"/>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B135" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C135" s="9"/>
+      <c r="D135" s="9"/>
+      <c r="E135" s="9"/>
+      <c r="F135" s="9"/>
+      <c r="G135" s="9"/>
+      <c r="H135" s="9"/>
+      <c r="I135" s="9"/>
+      <c r="J135" s="9"/>
+      <c r="K135" s="9"/>
+      <c r="L135" s="9"/>
+      <c r="M135" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>